<commit_message>
Add initial structure and electrolyser data
</commit_message>
<xml_diff>
--- a/VT_IE_SUP.xlsx
+++ b/VT_IE_SUP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6738FC0E-79D5-4A92-B8E6-031AC7684FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276B18F-9C90-4ED1-B637-830C6AE7EE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="23" r:id="rId1"/>
@@ -866,7 +866,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="633">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -2117,12 +2117,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>centralised</t>
-  </si>
-  <si>
-    <t>decentralised</t>
-  </si>
-  <si>
     <t>Methane - eNergy Emissions</t>
   </si>
   <si>
@@ -2851,6 +2845,24 @@
   </si>
   <si>
     <t>NCAP_BND~0</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>High pressure (500 bar)</t>
+  </si>
+  <si>
+    <t>Medium pressure (100 bar)</t>
+  </si>
+  <si>
+    <t>Centralised</t>
+  </si>
+  <si>
+    <t>Distributed</t>
   </si>
 </sst>
 </file>
@@ -7148,9 +7160,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7188,9 +7200,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7223,26 +7235,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7275,26 +7270,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7497,17 +7475,17 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -7932,7 +7910,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1">
       <c r="A16" s="440" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B16" s="440"/>
       <c r="C16" s="440"/>
@@ -8018,10 +7996,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1">
       <c r="A19" s="283" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B19" s="439" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C19" s="439"/>
       <c r="D19" s="439"/>
@@ -8050,10 +8028,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1">
       <c r="A20" s="283" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B20" s="439" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C20" s="439"/>
       <c r="D20" s="439"/>
@@ -8082,10 +8060,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1">
       <c r="A21" s="283" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B21" s="286" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C21" s="286"/>
       <c r="D21" s="286"/>
@@ -8142,10 +8120,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1">
       <c r="A23" s="283" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B23" s="439" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C23" s="439"/>
       <c r="D23" s="439"/>
@@ -8175,7 +8153,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1">
       <c r="A24" s="283"/>
       <c r="B24" s="286" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C24" s="286"/>
       <c r="D24" s="286"/>
@@ -8205,7 +8183,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1">
       <c r="A25" s="283"/>
       <c r="B25" s="286" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C25" s="286"/>
       <c r="D25" s="286"/>
@@ -8234,10 +8212,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1">
       <c r="A26" s="283" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B26" s="439" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C26" s="439"/>
       <c r="D26" s="439"/>
@@ -8322,7 +8300,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1">
       <c r="A29" s="283" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B29" s="287">
         <v>1</v>
@@ -8354,10 +8332,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1">
       <c r="A30" s="283" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B30" s="441" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C30" s="439"/>
       <c r="D30" s="439"/>
@@ -8386,10 +8364,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1">
       <c r="A31" s="283" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B31" s="439" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C31" s="439"/>
       <c r="D31" s="439"/>
@@ -8419,7 +8397,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1">
       <c r="A32" s="289"/>
       <c r="B32" s="290" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C32" s="289"/>
       <c r="D32" s="289"/>
@@ -10351,30 +10329,30 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
+    <col min="4" max="4" width="34.86328125" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.59765625" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.59765625" customWidth="1"/>
+    <col min="17" max="17" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="18.75">
+    <row r="2" spans="2:15" ht="18">
       <c r="B2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -10388,7 +10366,7 @@
     </row>
     <row r="3" spans="2:15">
       <c r="B3" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>2</v>
@@ -10409,13 +10387,13 @@
         <v>45</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="L3" s="12" t="s">
         <v>207</v>
@@ -10424,9 +10402,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15.75" thickBot="1">
+    <row r="4" spans="2:15" ht="14.65" thickBot="1">
       <c r="B4" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>46</v>
@@ -10638,10 +10616,10 @@
         <v>222</v>
       </c>
       <c r="J9" s="192" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="K9" s="192" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="L9" s="126" t="s">
         <v>221</v>
@@ -10694,7 +10672,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="18.75">
+    <row r="13" spans="2:15" ht="18">
       <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
@@ -10713,9 +10691,9 @@
       <c r="M13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="2:15" ht="25.5">
+    <row r="14" spans="2:15" ht="26.25">
       <c r="B14" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>2</v>
@@ -10743,9 +10721,9 @@
       <c r="N14" s="2"/>
       <c r="O14" s="105"/>
     </row>
-    <row r="15" spans="2:15" ht="15.75" thickBot="1">
+    <row r="15" spans="2:15" ht="14.65" thickBot="1">
       <c r="B15" s="8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>46</v>
@@ -10982,15 +10960,15 @@
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="40" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="274" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C29" s="272" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="30" spans="2:15">
@@ -11027,12 +11005,12 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
   </sheetData>
@@ -11055,21 +11033,21 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
-    <col min="2" max="2" width="12.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="69.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="22" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="22"/>
-    <col min="10" max="10" width="14.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.1328125" style="22"/>
+    <col min="2" max="2" width="12.86328125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="69.73046875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1328125" style="22" customWidth="1"/>
+    <col min="7" max="9" width="9.1328125" style="22"/>
+    <col min="10" max="10" width="14.1328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.59765625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="18.75">
+    <row r="2" spans="2:18" ht="18">
       <c r="B2" s="3" t="s">
         <v>131</v>
       </c>
@@ -11083,7 +11061,7 @@
     </row>
     <row r="3" spans="2:18">
       <c r="B3" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>2</v>
@@ -11103,7 +11081,7 @@
     </row>
     <row r="4" spans="2:18" ht="13.5" thickBot="1">
       <c r="B4" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>59</v>
@@ -11119,7 +11097,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="2:18" ht="15">
+    <row r="5" spans="2:18" ht="14.25">
       <c r="B5" s="21" t="str">
         <f>Processes!C51</f>
         <v>IE,National</v>
@@ -11144,7 +11122,7 @@
       </c>
       <c r="R5" s="23"/>
     </row>
-    <row r="6" spans="2:18" ht="15">
+    <row r="6" spans="2:18" ht="14.25">
       <c r="B6" s="21" t="str">
         <f>Processes!C54</f>
         <v>IE,National</v>
@@ -11167,7 +11145,7 @@
       <c r="G6" s="452"/>
       <c r="R6" s="23"/>
     </row>
-    <row r="7" spans="2:18" ht="15">
+    <row r="7" spans="2:18" ht="14.25">
       <c r="B7" s="21" t="str">
         <f>Processes!C60</f>
         <v>IE,National</v>
@@ -11190,7 +11168,7 @@
       <c r="G7" s="452"/>
       <c r="R7" s="23"/>
     </row>
-    <row r="8" spans="2:18" ht="15">
+    <row r="8" spans="2:18" ht="14.25">
       <c r="B8" s="21" t="str">
         <f>Processes!C66</f>
         <v>IE,National</v>
@@ -11213,7 +11191,7 @@
       <c r="G8" s="452"/>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="2:18" ht="15">
+    <row r="9" spans="2:18" ht="14.25">
       <c r="B9" s="21" t="str">
         <f>Processes!C69</f>
         <v>IE,National</v>
@@ -11236,7 +11214,7 @@
       <c r="G9" s="452"/>
       <c r="R9" s="23"/>
     </row>
-    <row r="10" spans="2:18" ht="15">
+    <row r="10" spans="2:18" ht="14.25">
       <c r="B10" s="21" t="str">
         <f>Processes!C57</f>
         <v>IE,National</v>
@@ -11259,7 +11237,7 @@
       <c r="G10" s="452"/>
       <c r="R10" s="23"/>
     </row>
-    <row r="11" spans="2:18" ht="15">
+    <row r="11" spans="2:18" ht="14.25">
       <c r="B11" s="21" t="str">
         <f>Processes!C72</f>
         <v>IE,National</v>
@@ -11282,7 +11260,7 @@
       <c r="G11" s="452"/>
       <c r="R11" s="23"/>
     </row>
-    <row r="12" spans="2:18" ht="15">
+    <row r="12" spans="2:18" ht="14.25">
       <c r="B12" s="21" t="str">
         <f>Processes!C75</f>
         <v>IE,National</v>
@@ -11305,7 +11283,7 @@
       <c r="G12" s="452"/>
       <c r="R12" s="23"/>
     </row>
-    <row r="13" spans="2:18" ht="15">
+    <row r="13" spans="2:18" ht="14.25">
       <c r="B13" s="21" t="str">
         <f>Processes!C63</f>
         <v>IE,National</v>
@@ -11328,7 +11306,7 @@
       <c r="G13" s="452"/>
       <c r="R13" s="23"/>
     </row>
-    <row r="14" spans="2:18" ht="15">
+    <row r="14" spans="2:18" ht="14.25">
       <c r="B14" s="45" t="str">
         <f>Processes!C78</f>
         <v>IE,National</v>
@@ -11351,7 +11329,7 @@
       <c r="G14" s="452"/>
       <c r="R14" s="23"/>
     </row>
-    <row r="15" spans="2:18" ht="15">
+    <row r="15" spans="2:18" ht="14.25">
       <c r="B15" s="21" t="str">
         <f>Processes!C52</f>
         <v>IE,National</v>
@@ -11374,7 +11352,7 @@
       <c r="G15" s="452"/>
       <c r="R15" s="23"/>
     </row>
-    <row r="16" spans="2:18" ht="15">
+    <row r="16" spans="2:18" ht="14.25">
       <c r="B16" s="21" t="str">
         <f>Processes!C55</f>
         <v>IE,National</v>
@@ -11397,7 +11375,7 @@
       <c r="G16" s="452"/>
       <c r="R16" s="23"/>
     </row>
-    <row r="17" spans="2:18" ht="15">
+    <row r="17" spans="2:18" ht="14.25">
       <c r="B17" s="21" t="str">
         <f>Processes!C61</f>
         <v>IE,National</v>
@@ -11420,7 +11398,7 @@
       <c r="G17" s="452"/>
       <c r="R17" s="23"/>
     </row>
-    <row r="18" spans="2:18" ht="15">
+    <row r="18" spans="2:18" ht="14.25">
       <c r="B18" s="21" t="str">
         <f>Processes!C67</f>
         <v>IE,National</v>
@@ -11443,7 +11421,7 @@
       <c r="G18" s="452"/>
       <c r="R18" s="23"/>
     </row>
-    <row r="19" spans="2:18" ht="15">
+    <row r="19" spans="2:18" ht="14.25">
       <c r="B19" s="21" t="str">
         <f>Processes!C70</f>
         <v>IE,National</v>
@@ -11466,7 +11444,7 @@
       <c r="G19" s="452"/>
       <c r="R19" s="23"/>
     </row>
-    <row r="20" spans="2:18" ht="15">
+    <row r="20" spans="2:18" ht="14.25">
       <c r="B20" s="21" t="str">
         <f>Processes!C58</f>
         <v>IE,National</v>
@@ -11809,7 +11787,7 @@
       <c r="F36" s="50"/>
       <c r="G36" s="190"/>
     </row>
-    <row r="37" spans="2:7" ht="15">
+    <row r="37" spans="2:7" ht="14.25">
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
@@ -11817,7 +11795,7 @@
       <c r="F37"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="2:7" ht="15">
+    <row r="38" spans="2:7" ht="14.25">
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
@@ -11825,7 +11803,7 @@
       <c r="F38"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="2:7" ht="15">
+    <row r="39" spans="2:7" ht="14.25">
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
@@ -11833,7 +11811,7 @@
       <c r="F39"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="2:7" ht="15">
+    <row r="40" spans="2:7" ht="14.25">
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
@@ -11841,7 +11819,7 @@
       <c r="F40"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="2:7" ht="15">
+    <row r="41" spans="2:7" ht="14.25">
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
@@ -11849,7 +11827,7 @@
       <c r="F41"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="2:7" ht="15">
+    <row r="42" spans="2:7" ht="14.25">
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
@@ -11875,21 +11853,21 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="9.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="9.73046875" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" style="23" customWidth="1"/>
     <col min="4" max="4" width="17" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="23"/>
-    <col min="7" max="20" width="9.42578125" style="25" customWidth="1"/>
-    <col min="21" max="23" width="9.42578125" style="23" customWidth="1"/>
-    <col min="24" max="24" width="28.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="23"/>
-    <col min="26" max="26" width="13.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" style="23"/>
+    <col min="7" max="20" width="9.3984375" style="25" customWidth="1"/>
+    <col min="21" max="23" width="9.3984375" style="23" customWidth="1"/>
+    <col min="24" max="24" width="28.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.1328125" style="23"/>
+    <col min="26" max="26" width="13.59765625" style="23" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" style="23" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="23"/>
+    <col min="28" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:26">
@@ -11897,7 +11875,7 @@
       <c r="S1" s="23"/>
       <c r="T1" s="23"/>
     </row>
-    <row r="2" spans="2:26" ht="18.75">
+    <row r="2" spans="2:26" ht="18">
       <c r="B2" s="112" t="s">
         <v>145</v>
       </c>
@@ -11905,7 +11883,7 @@
       <c r="D2" s="113"/>
       <c r="E2" s="114"/>
       <c r="F2" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G2" s="120"/>
       <c r="H2" s="121"/>
@@ -11922,9 +11900,9 @@
       <c r="S2" s="124"/>
       <c r="T2" s="23"/>
     </row>
-    <row r="3" spans="2:26" ht="25.5">
+    <row r="3" spans="2:26" ht="26.25">
       <c r="B3" s="110" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C3" s="110" t="s">
         <v>2</v>
@@ -11939,19 +11917,19 @@
         <v>38</v>
       </c>
       <c r="G3" s="109" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H3" s="109" t="s">
         <v>219</v>
       </c>
       <c r="I3" s="109" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J3" s="109" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="K3" s="109" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="L3" s="109" t="s">
         <v>207</v>
@@ -12462,7 +12440,7 @@
     </row>
     <row r="22" spans="3:30">
       <c r="C22" s="23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D22" s="224">
         <f>1/SUM(E24:E35)</f>
@@ -12648,36 +12626,36 @@
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="13.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="13.3984375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="46.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.73046875" style="23" customWidth="1"/>
     <col min="6" max="6" width="10" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="9.265625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" style="23" customWidth="1"/>
     <col min="10" max="10" width="11" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="10.140625" style="23" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="10.28515625" style="23" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="23"/>
+    <col min="11" max="15" width="10.1328125" style="23" customWidth="1"/>
+    <col min="16" max="16" width="9.73046875" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="10.265625" style="23" customWidth="1"/>
+    <col min="22" max="22" width="9.1328125" style="23"/>
     <col min="23" max="23" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="23"/>
+    <col min="24" max="24" width="26.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="18.75">
+    <row r="2" spans="2:20" ht="18">
       <c r="B2" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="G2" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -12687,7 +12665,7 @@
     </row>
     <row r="3" spans="2:20">
       <c r="B3" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>2</v>
@@ -12702,16 +12680,16 @@
         <v>38</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>40</v>
@@ -12729,16 +12707,16 @@
         <v>45</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="R3"/>
     </row>
-    <row r="4" spans="2:20" ht="15.75" thickBot="1">
+    <row r="4" spans="2:20" ht="14.65" thickBot="1">
       <c r="B4" s="13" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>46</v>
@@ -13549,11 +13527,11 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="18.85546875" style="23" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="18.86328125" style="23" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13570,7 +13548,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1">
       <c r="B5" s="163" t="s">
         <v>16</v>
       </c>
@@ -13666,9 +13644,9 @@
       <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.3984375" customWidth="1"/>
     <col min="2" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13713,7 +13691,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+    <row r="3" spans="1:22" ht="14.65" thickBot="1">
       <c r="A3" s="69" t="s">
         <v>92</v>
       </c>
@@ -13748,7 +13726,7 @@
       </c>
       <c r="Q4" s="23"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1">
+    <row r="5" spans="1:22" ht="14.65" thickBot="1">
       <c r="A5" s="75" t="s">
         <v>96</v>
       </c>
@@ -13758,7 +13736,7 @@
       </c>
       <c r="J5" s="23"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" thickBot="1">
+    <row r="6" spans="1:22" ht="14.65" thickBot="1">
       <c r="A6" s="77"/>
       <c r="B6" s="78" t="s">
         <v>18</v>
@@ -13801,7 +13779,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15.75" thickBot="1">
+    <row r="7" spans="1:22" ht="14.65" thickBot="1">
       <c r="A7" s="80" t="s">
         <v>98</v>
       </c>
@@ -13854,7 +13832,7 @@
       <c r="R7" s="84"/>
       <c r="S7" s="84"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1">
+    <row r="8" spans="1:22" ht="14.65" thickBot="1">
       <c r="A8" s="80" t="s">
         <v>98</v>
       </c>
@@ -13907,7 +13885,7 @@
       <c r="R8" s="84"/>
       <c r="S8" s="84"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" thickBot="1">
+    <row r="9" spans="1:22" ht="14.65" thickBot="1">
       <c r="A9" s="80" t="s">
         <v>103</v>
       </c>
@@ -13960,7 +13938,7 @@
       <c r="R9" s="84"/>
       <c r="S9" s="84"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1">
+    <row r="10" spans="1:22" ht="14.65" thickBot="1">
       <c r="A10" s="80" t="s">
         <v>103</v>
       </c>
@@ -14013,7 +13991,7 @@
       <c r="R10" s="84"/>
       <c r="S10" s="84"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1">
+    <row r="11" spans="1:22" ht="14.65" thickBot="1">
       <c r="A11" s="80" t="s">
         <v>83</v>
       </c>
@@ -14060,7 +14038,7 @@
         <v>5.4816516360000005</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1">
+    <row r="12" spans="1:22" ht="14.65" thickBot="1">
       <c r="A12" s="80" t="s">
         <v>83</v>
       </c>
@@ -14107,7 +14085,7 @@
         <v>13.781408235406515</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1">
+    <row r="13" spans="1:22" ht="14.65" thickBot="1">
       <c r="A13" s="80" t="s">
         <v>84</v>
       </c>
@@ -14154,7 +14132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1">
+    <row r="14" spans="1:22" ht="14.65" thickBot="1">
       <c r="A14" s="80" t="s">
         <v>84</v>
       </c>
@@ -14207,7 +14185,7 @@
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" thickBot="1">
+    <row r="16" spans="1:22" ht="14.65" thickBot="1">
       <c r="A16" s="75" t="s">
         <v>100</v>
       </c>
@@ -14223,7 +14201,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15.75" thickBot="1">
+    <row r="17" spans="1:26" ht="14.65" thickBot="1">
       <c r="A17" s="77"/>
       <c r="B17" s="78" t="s">
         <v>18</v>
@@ -14293,7 +14271,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15.75" thickBot="1">
+    <row r="18" spans="1:26" ht="14.65" thickBot="1">
       <c r="A18" s="80" t="s">
         <v>98</v>
       </c>
@@ -14342,7 +14320,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="87"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" thickBot="1">
+    <row r="19" spans="1:26" ht="14.65" thickBot="1">
       <c r="A19" s="80" t="s">
         <v>98</v>
       </c>
@@ -14429,7 +14407,7 @@
         <v>2.6576562288177672</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" thickBot="1">
+    <row r="20" spans="1:26" ht="14.65" thickBot="1">
       <c r="A20" s="80" t="s">
         <v>103</v>
       </c>
@@ -14476,7 +14454,7 @@
         <v>144.52992698400001</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15.75" thickBot="1">
+    <row r="21" spans="1:26" ht="14.65" thickBot="1">
       <c r="A21" s="80" t="s">
         <v>103</v>
       </c>
@@ -14563,7 +14541,7 @@
         <v>5.4463236801828891</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="15.75" thickBot="1">
+    <row r="22" spans="1:26" ht="14.65" thickBot="1">
       <c r="A22" s="80" t="s">
         <v>83</v>
       </c>
@@ -14611,7 +14589,7 @@
       </c>
       <c r="P22" s="87"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" thickBot="1">
+    <row r="23" spans="1:26" ht="14.65" thickBot="1">
       <c r="A23" s="80" t="s">
         <v>83</v>
       </c>
@@ -14698,7 +14676,7 @@
         <v>12.446066141998699</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15.75" thickBot="1">
+    <row r="24" spans="1:26" ht="14.65" thickBot="1">
       <c r="A24" s="80" t="s">
         <v>84</v>
       </c>
@@ -14745,7 +14723,7 @@
         <v>3.8660492520000003</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" thickBot="1">
+    <row r="25" spans="1:26" ht="14.65" thickBot="1">
       <c r="A25" s="80" t="s">
         <v>84</v>
       </c>
@@ -14832,7 +14810,7 @@
         <v>24.555246283161342</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15.75" thickBot="1">
+    <row r="26" spans="1:26" ht="14.65" thickBot="1">
       <c r="A26" s="75" t="s">
         <v>102</v>
       </c>
@@ -14849,7 +14827,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="15.75" thickBot="1">
+    <row r="27" spans="1:26" ht="14.65" thickBot="1">
       <c r="A27" s="90"/>
       <c r="B27" s="78" t="s">
         <v>18</v>
@@ -14919,7 +14897,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15.75" thickBot="1">
+    <row r="28" spans="1:26" ht="14.65" thickBot="1">
       <c r="A28" s="80" t="s">
         <v>98</v>
       </c>
@@ -14967,7 +14945,7 @@
       </c>
       <c r="P28" s="87"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" thickBot="1">
+    <row r="29" spans="1:26" ht="14.65" thickBot="1">
       <c r="A29" s="80" t="s">
         <v>98</v>
       </c>
@@ -15054,7 +15032,7 @@
         <v>3.425007675166559</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15.75" thickBot="1">
+    <row r="30" spans="1:26" ht="14.65" thickBot="1">
       <c r="A30" s="80" t="s">
         <v>103</v>
       </c>
@@ -15101,7 +15079,7 @@
         <v>236.79263826000002</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="15.75" thickBot="1">
+    <row r="31" spans="1:26" ht="14.65" thickBot="1">
       <c r="A31" s="80" t="s">
         <v>103</v>
       </c>
@@ -15188,7 +15166,7 @@
         <v>6.8687312392684552</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="15.75" thickBot="1">
+    <row r="32" spans="1:26" ht="14.65" thickBot="1">
       <c r="A32" s="80" t="s">
         <v>83</v>
       </c>
@@ -15236,7 +15214,7 @@
       </c>
       <c r="P32" s="87"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" thickBot="1">
+    <row r="33" spans="1:26" ht="14.65" thickBot="1">
       <c r="A33" s="80" t="s">
         <v>83</v>
       </c>
@@ -15323,7 +15301,7 @@
         <v>14.991427037204447</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15.75" thickBot="1">
+    <row r="34" spans="1:26" ht="14.65" thickBot="1">
       <c r="A34" s="80" t="s">
         <v>84</v>
       </c>
@@ -15370,7 +15348,7 @@
         <v>4.3794765360000003</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="15.75" thickBot="1">
+    <row r="35" spans="1:26" ht="14.65" thickBot="1">
       <c r="A35" s="80" t="s">
         <v>84</v>
       </c>
@@ -15467,7 +15445,7 @@
       <c r="M36" s="57"/>
       <c r="N36" s="57"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" thickBot="1">
+    <row r="37" spans="1:26" ht="14.65" thickBot="1">
       <c r="A37" s="75" t="s">
         <v>104</v>
       </c>
@@ -15487,7 +15465,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="15.75" thickBot="1">
+    <row r="38" spans="1:26" ht="14.65" thickBot="1">
       <c r="A38" s="77"/>
       <c r="B38" s="78" t="s">
         <v>18</v>
@@ -15557,7 +15535,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="15.75" thickBot="1">
+    <row r="39" spans="1:26" ht="14.65" thickBot="1">
       <c r="A39" s="80" t="s">
         <v>98</v>
       </c>
@@ -15605,7 +15583,7 @@
       </c>
       <c r="P39" s="87"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" thickBot="1">
+    <row r="40" spans="1:26" ht="14.65" thickBot="1">
       <c r="A40" s="80" t="s">
         <v>98</v>
       </c>
@@ -15692,7 +15670,7 @@
         <v>3.0319740075244952</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="15.75" thickBot="1">
+    <row r="41" spans="1:26" ht="14.65" thickBot="1">
       <c r="A41" s="80" t="s">
         <v>103</v>
       </c>
@@ -15739,7 +15717,7 @@
         <v>17.883748728000004</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="15.75" thickBot="1">
+    <row r="42" spans="1:26" ht="14.65" thickBot="1">
       <c r="A42" s="80" t="s">
         <v>103</v>
       </c>
@@ -15826,7 +15804,7 @@
         <v>6.1949592375963451</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="15.75" thickBot="1">
+    <row r="43" spans="1:26" ht="14.65" thickBot="1">
       <c r="A43" s="80" t="s">
         <v>83</v>
       </c>
@@ -15874,7 +15852,7 @@
       </c>
       <c r="P43" s="87"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" thickBot="1">
+    <row r="44" spans="1:26" ht="14.65" thickBot="1">
       <c r="A44" s="80" t="s">
         <v>83</v>
       </c>
@@ -15961,7 +15939,7 @@
         <v>18.45386649024168</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="15.75" thickBot="1">
+    <row r="45" spans="1:26" ht="14.65" thickBot="1">
       <c r="A45" s="80" t="s">
         <v>84</v>
       </c>
@@ -16008,7 +15986,7 @@
         <v>4.602800448</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="15.75" thickBot="1">
+    <row r="46" spans="1:26" ht="14.65" thickBot="1">
       <c r="A46" s="80" t="s">
         <v>84</v>
       </c>
@@ -16105,7 +16083,7 @@
       <c r="M47" s="57"/>
       <c r="N47" s="57"/>
     </row>
-    <row r="48" spans="1:26" ht="15.75" thickBot="1">
+    <row r="48" spans="1:26" ht="14.65" thickBot="1">
       <c r="A48" s="75" t="s">
         <v>105</v>
       </c>
@@ -16125,7 +16103,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="15.75" thickBot="1">
+    <row r="49" spans="1:26" ht="14.65" thickBot="1">
       <c r="A49" s="77"/>
       <c r="B49" s="78" t="s">
         <v>18</v>
@@ -16195,7 +16173,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="15.75" thickBot="1">
+    <row r="50" spans="1:26" ht="14.65" thickBot="1">
       <c r="A50" s="80" t="s">
         <v>98</v>
       </c>
@@ -16243,7 +16221,7 @@
       </c>
       <c r="P50" s="87"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" thickBot="1">
+    <row r="51" spans="1:26" ht="14.65" thickBot="1">
       <c r="A51" s="80" t="s">
         <v>98</v>
       </c>
@@ -16330,7 +16308,7 @@
         <v>3.949052565355978</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="15.75" thickBot="1">
+    <row r="52" spans="1:26" ht="14.65" thickBot="1">
       <c r="A52" s="80" t="s">
         <v>103</v>
       </c>
@@ -16377,7 +16355,7 @@
         <v>110.14646000400001</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="15.75" thickBot="1">
+    <row r="53" spans="1:26" ht="14.65" thickBot="1">
       <c r="A53" s="80" t="s">
         <v>103</v>
       </c>
@@ -16464,7 +16442,7 @@
         <v>7.8793892417766198</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="15.75" thickBot="1">
+    <row r="54" spans="1:26" ht="14.65" thickBot="1">
       <c r="A54" s="80" t="s">
         <v>83</v>
       </c>
@@ -16512,7 +16490,7 @@
       </c>
       <c r="P54" s="87"/>
     </row>
-    <row r="55" spans="1:26" ht="15.75" thickBot="1">
+    <row r="55" spans="1:26" ht="14.65" thickBot="1">
       <c r="A55" s="80" t="s">
         <v>83</v>
       </c>
@@ -16599,7 +16577,7 @@
         <v>22.533930278145014</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="15.75" thickBot="1">
+    <row r="56" spans="1:26" ht="14.65" thickBot="1">
       <c r="A56" s="80" t="s">
         <v>84</v>
       </c>
@@ -16646,7 +16624,7 @@
         <v>5.1162277320000005</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="15.75" thickBot="1">
+    <row r="57" spans="1:26" ht="14.65" thickBot="1">
       <c r="A57" s="80" t="s">
         <v>84</v>
       </c>
@@ -16753,14 +16731,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="66" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B1" s="66"/>
     </row>
@@ -16769,7 +16747,7 @@
         <v>93</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C2" s="23">
         <v>4.1868000000000002E-2</v>
@@ -16780,10 +16758,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="23" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C3" s="23">
         <v>1.0550999999999999</v>
@@ -16797,22 +16775,22 @@
         <v>89</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C4" s="23">
         <v>7.33</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E4" s="255"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="23" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C5" s="23">
         <f>C2/C4*1000</f>
@@ -16824,35 +16802,35 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="66" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="23" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C10" s="23">
         <v>1.1194745098039223</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C11" s="23">
         <v>1.1809545098039216</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -16870,35 +16848,35 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" customWidth="1"/>
+    <col min="3" max="3" width="3.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.73046875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.59765625" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:30">
@@ -17022,13 +17000,13 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="228" t="s">
+        <v>453</v>
+      </c>
+      <c r="D5" s="228" t="s">
         <v>454</v>
-      </c>
-      <c r="C5" s="228" t="s">
-        <v>455</v>
-      </c>
-      <c r="D5" s="228" t="s">
-        <v>456</v>
       </c>
       <c r="E5" s="227" t="str">
         <f>A11</f>
@@ -17137,7 +17115,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C6" s="227" t="str">
         <f>C5</f>
@@ -17254,7 +17232,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C7" s="227" t="str">
         <f>"*"&amp;C5</f>
@@ -17369,225 +17347,225 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1">
+    <row r="10" spans="1:30" ht="14.65" thickBot="1">
       <c r="A10" s="229" t="s">
         <v>279</v>
       </c>
       <c r="B10" s="229" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="230" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B11" s="230" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="31" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="31" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="31" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="31" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="31" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="31" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="31" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="31" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="31" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="31" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="31" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="31" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="31" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="31" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="31" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="31" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="31" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="31" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="31" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="31" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="31" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="31" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="31" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="31" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="31" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="231" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -17641,52 +17619,52 @@
       <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="133" customWidth="1"/>
+    <col min="1" max="1" width="38.1328125" style="133" customWidth="1"/>
     <col min="2" max="2" width="13" style="131" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.5703125" style="134" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="134"/>
-    <col min="6" max="6" width="6.140625" style="135" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="135" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="134" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="135" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.59765625" style="134" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" style="134"/>
+    <col min="6" max="6" width="6.1328125" style="135" customWidth="1"/>
+    <col min="7" max="7" width="5.86328125" style="135" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="134" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1328125" style="135" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="135" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" style="135" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="132" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="131" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="131" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" style="131" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="131" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="131" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="131" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="131" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="5.42578125" style="131" customWidth="1"/>
-    <col min="26" max="26" width="5.42578125" style="135" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="132" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" style="132" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="5.5703125" style="131" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="131" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7109375" style="131" customWidth="1"/>
-    <col min="33" max="33" width="5.5703125" style="131" customWidth="1"/>
-    <col min="34" max="34" width="5.85546875" style="131" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.86328125" style="135" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.73046875" style="132" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1328125" style="131" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1328125" style="131" customWidth="1"/>
+    <col min="15" max="15" width="5.265625" style="131" customWidth="1"/>
+    <col min="16" max="16" width="7.3984375" style="131" customWidth="1"/>
+    <col min="17" max="17" width="7.3984375" style="131" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1328125" style="131" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.265625" style="131" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.3984375" style="131" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.3984375" style="131" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.86328125" style="131" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="5.3984375" style="131" customWidth="1"/>
+    <col min="26" max="26" width="5.3984375" style="135" customWidth="1"/>
+    <col min="27" max="27" width="8.1328125" style="132" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.73046875" style="132" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="5.59765625" style="131" customWidth="1"/>
+    <col min="31" max="31" width="8.73046875" style="131" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.73046875" style="131" customWidth="1"/>
+    <col min="33" max="33" width="5.59765625" style="131" customWidth="1"/>
+    <col min="34" max="34" width="5.86328125" style="131" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="7" style="131" customWidth="1"/>
-    <col min="37" max="40" width="5.5703125" style="131" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" style="132" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.42578125" style="132" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" style="131" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="131"/>
+    <col min="37" max="40" width="5.59765625" style="131" customWidth="1"/>
+    <col min="41" max="41" width="8.73046875" style="132" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.3984375" style="132" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.265625" style="131" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.1328125" style="131"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="98.25" thickBot="1">
+    <row r="1" spans="1:43" ht="96" thickBot="1">
       <c r="A1" s="212" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B1" s="211" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C1" s="213" t="s">
         <v>160</v>
@@ -17722,7 +17700,7 @@
         <v>170</v>
       </c>
       <c r="N1" s="220" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O1" s="209" t="s">
         <v>171</v>
@@ -17773,10 +17751,10 @@
         <v>186</v>
       </c>
       <c r="AE1" s="221" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="AF1" s="218" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AG1" s="209" t="s">
         <v>187</v>
@@ -17785,19 +17763,19 @@
         <v>188</v>
       </c>
       <c r="AI1" s="221" t="s">
+        <v>444</v>
+      </c>
+      <c r="AJ1" s="218" t="s">
+        <v>445</v>
+      </c>
+      <c r="AK1" s="221" t="s">
         <v>446</v>
       </c>
-      <c r="AJ1" s="218" t="s">
+      <c r="AL1" s="218" t="s">
         <v>447</v>
       </c>
-      <c r="AK1" s="221" t="s">
+      <c r="AM1" s="219" t="s">
         <v>448</v>
-      </c>
-      <c r="AL1" s="218" t="s">
-        <v>449</v>
-      </c>
-      <c r="AM1" s="219" t="s">
-        <v>450</v>
       </c>
       <c r="AN1" s="210" t="s">
         <v>189</v>
@@ -18804,7 +18782,7 @@
     </row>
     <row r="10" spans="1:43">
       <c r="A10" s="358" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B10" s="359"/>
       <c r="C10" s="360">
@@ -18886,7 +18864,7 @@
     </row>
     <row r="11" spans="1:43">
       <c r="A11" s="307" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B11" s="308"/>
       <c r="C11" s="309">
@@ -18966,7 +18944,7 @@
     </row>
     <row r="12" spans="1:43">
       <c r="A12" s="307" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B12" s="308"/>
       <c r="C12" s="309"/>
@@ -19018,7 +18996,7 @@
     </row>
     <row r="13" spans="1:43">
       <c r="A13" s="307" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B13" s="308"/>
       <c r="C13" s="309">
@@ -19082,7 +19060,7 @@
     </row>
     <row r="14" spans="1:43">
       <c r="A14" s="371" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B14" s="372"/>
       <c r="C14" s="373">
@@ -19322,7 +19300,7 @@
     </row>
     <row r="16" spans="1:43">
       <c r="A16" s="358" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B16" s="359"/>
       <c r="C16" s="360">
@@ -19386,7 +19364,7 @@
     </row>
     <row r="17" spans="1:43">
       <c r="A17" s="307" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B17" s="308"/>
       <c r="C17" s="309">
@@ -19450,7 +19428,7 @@
     </row>
     <row r="18" spans="1:43">
       <c r="A18" s="307" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B18" s="308"/>
       <c r="C18" s="309"/>
@@ -19502,7 +19480,7 @@
     </row>
     <row r="19" spans="1:43">
       <c r="A19" s="307" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B19" s="308"/>
       <c r="C19" s="309"/>
@@ -19563,7 +19541,7 @@
     </row>
     <row r="20" spans="1:43">
       <c r="A20" s="371" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B20" s="372"/>
       <c r="C20" s="373"/>
@@ -19808,7 +19786,7 @@
     </row>
     <row r="22" spans="1:43">
       <c r="A22" s="358" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B22" s="359"/>
       <c r="C22" s="409"/>
@@ -19872,7 +19850,7 @@
     </row>
     <row r="23" spans="1:43">
       <c r="A23" s="413" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B23" s="384"/>
       <c r="C23" s="414"/>
@@ -19922,7 +19900,7 @@
     </row>
     <row r="24" spans="1:43" ht="13.5" thickBot="1">
       <c r="A24" s="322" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B24" s="323"/>
       <c r="C24" s="423">
@@ -20268,46 +20246,46 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:AC86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="O2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7:AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="85.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.59765625" customWidth="1"/>
+    <col min="2" max="2" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.86328125" customWidth="1"/>
+    <col min="6" max="6" width="85.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.59765625" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.59765625" customWidth="1"/>
+    <col min="16" max="16" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.5703125" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.5703125" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.5703125" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="1.5703125" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.59765625" customWidth="1"/>
+    <col min="20" max="20" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.59765625" customWidth="1"/>
+    <col min="22" max="22" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="1.59765625" customWidth="1"/>
+    <col min="26" max="26" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="1.59765625" customWidth="1"/>
+    <col min="29" max="29" width="15.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:29" ht="18.75">
+    <row r="3" spans="2:29" ht="18">
       <c r="B3" s="165" t="s">
         <v>282</v>
       </c>
       <c r="E3" s="165" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L3" t="s">
         <v>358</v>
@@ -20322,7 +20300,7 @@
         <v>377</v>
       </c>
       <c r="V3" s="165" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Y3" s="165" t="s">
         <v>384</v>
@@ -20331,7 +20309,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="2:29" ht="15.75" thickBot="1">
+    <row r="4" spans="2:29" ht="14.65" thickBot="1">
       <c r="B4" s="166" t="s">
         <v>279</v>
       </c>
@@ -20431,7 +20409,7 @@
         <v>338</v>
       </c>
       <c r="N5" s="167" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="P5" s="167" t="s">
         <v>335</v>
@@ -20443,13 +20421,13 @@
         <v>9</v>
       </c>
       <c r="T5" s="167" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="V5" s="167" t="s">
         <v>378</v>
       </c>
       <c r="W5" s="167" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y5" s="167" t="s">
         <v>382</v>
@@ -20458,10 +20436,10 @@
         <v>385</v>
       </c>
       <c r="AB5" s="167" t="s">
-        <v>388</v>
+        <v>627</v>
       </c>
       <c r="AC5" s="167" t="s">
-        <v>390</v>
+        <v>629</v>
       </c>
     </row>
     <row r="6" spans="2:29">
@@ -20499,7 +20477,7 @@
         <v>367</v>
       </c>
       <c r="N6" s="167" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="P6" s="167" t="s">
         <v>281</v>
@@ -20511,13 +20489,13 @@
         <v>13</v>
       </c>
       <c r="T6" s="167" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="V6" s="167" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="W6" s="167" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="Y6" s="167" t="s">
         <v>383</v>
@@ -20526,10 +20504,10 @@
         <v>386</v>
       </c>
       <c r="AB6" s="167" t="s">
-        <v>389</v>
+        <v>628</v>
       </c>
       <c r="AC6" s="167" t="s">
-        <v>391</v>
+        <v>630</v>
       </c>
     </row>
     <row r="7" spans="2:29">
@@ -20567,7 +20545,7 @@
         <v>339</v>
       </c>
       <c r="N7" s="167" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="P7" s="167"/>
       <c r="Q7" s="167"/>
@@ -20575,16 +20553,20 @@
         <v>62</v>
       </c>
       <c r="T7" s="167" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="V7" s="167" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="W7" s="167"/>
       <c r="Y7" s="167"/>
       <c r="Z7" s="167"/>
-      <c r="AB7" s="167"/>
-      <c r="AC7" s="167"/>
+      <c r="AB7" s="167" t="s">
+        <v>388</v>
+      </c>
+      <c r="AC7" s="167" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="8" spans="2:29">
       <c r="B8" s="167" t="s">
@@ -20618,24 +20600,30 @@
         <v>13</v>
       </c>
       <c r="M8" s="167" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="N8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="P8" s="167"/>
       <c r="Q8" s="167"/>
       <c r="S8" s="167" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="T8" s="167" t="s">
+        <v>422</v>
+      </c>
+      <c r="V8" t="s">
         <v>424</v>
       </c>
-      <c r="V8" t="s">
-        <v>426</v>
-      </c>
       <c r="W8" t="s">
-        <v>427</v>
+        <v>425</v>
+      </c>
+      <c r="AB8" s="167" t="s">
+        <v>389</v>
+      </c>
+      <c r="AC8" s="167" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="9" spans="2:29">
@@ -20676,16 +20664,16 @@
         <v>363</v>
       </c>
       <c r="S9" s="167" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="T9" s="167" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="V9" s="167" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="W9" s="167" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="2:29">
@@ -20728,10 +20716,10 @@
       <c r="S10" s="167"/>
       <c r="T10" s="167"/>
       <c r="V10" s="167" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="W10" s="167" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="2:29">
@@ -20772,10 +20760,10 @@
         <v>376</v>
       </c>
       <c r="V11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="W11" s="167" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="2:29">
@@ -20816,10 +20804,10 @@
         <v>362</v>
       </c>
       <c r="V12" s="167" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="W12" s="167" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="2:29">
@@ -22507,10 +22495,10 @@
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="181" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C61" s="167" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E61" s="167" t="str">
         <f t="shared" si="16"/>
@@ -22650,7 +22638,7 @@
         <v>72</v>
       </c>
       <c r="C65" s="167" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E65" s="167" t="str">
         <f t="shared" si="16"/>
@@ -22752,10 +22740,10 @@
     </row>
     <row r="68" spans="2:11">
       <c r="B68" s="201" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C68" s="202" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E68" s="167" t="str">
         <f t="shared" ref="E68:E76" si="17">I68&amp;H68&amp;J68</f>
@@ -22790,7 +22778,7 @@
         <v>132</v>
       </c>
       <c r="C69" s="167" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E69" s="167" t="str">
         <f t="shared" si="17"/>
@@ -22822,10 +22810,10 @@
     </row>
     <row r="70" spans="2:11">
       <c r="B70" s="181" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C70" s="167" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E70" s="167" t="str">
         <f t="shared" si="17"/>
@@ -22857,10 +22845,10 @@
     </row>
     <row r="71" spans="2:11">
       <c r="B71" s="181" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C71" s="167" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E71" s="167" t="str">
         <f t="shared" si="17"/>
@@ -22892,10 +22880,10 @@
     </row>
     <row r="72" spans="2:11">
       <c r="B72" s="181" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C72" s="167" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E72" s="167" t="str">
         <f t="shared" si="17"/>
@@ -23267,10 +23255,10 @@
     </row>
     <row r="83" spans="2:11">
       <c r="B83" s="182" t="s">
+        <v>434</v>
+      </c>
+      <c r="C83" s="167" t="s">
         <v>436</v>
-      </c>
-      <c r="C83" s="167" t="s">
-        <v>438</v>
       </c>
       <c r="E83" s="167" t="str">
         <f>I83&amp;$P$5&amp;H83&amp;J83</f>
@@ -23298,10 +23286,10 @@
     </row>
     <row r="84" spans="2:11">
       <c r="B84" s="181" t="s">
+        <v>435</v>
+      </c>
+      <c r="C84" s="167" t="s">
         <v>437</v>
-      </c>
-      <c r="C84" s="167" t="s">
-        <v>439</v>
       </c>
       <c r="E84" s="167" t="str">
         <f>I84&amp;$P$5&amp;H84&amp;J84</f>
@@ -23388,15 +23376,15 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -23411,7 +23399,7 @@
       <c r="H2" s="170"/>
       <c r="I2" s="170"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1">
+    <row r="3" spans="2:9" ht="14.65" thickBot="1">
       <c r="B3" s="166" t="s">
         <v>15</v>
       </c>
@@ -24078,7 +24066,7 @@
         <v>BIOJKR</v>
       </c>
       <c r="D36" s="204" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E36" s="174" t="s">
         <v>10</v>
@@ -24495,12 +24483,12 @@
         <v>23</v>
       </c>
       <c r="C57" s="179" t="str">
-        <f>CONVENTIONS!$B$35&amp;CONVENTIONS!AB5</f>
+        <f>CONVENTIONS!$B$35&amp;CONVENTIONS!AB7</f>
         <v>ELCC</v>
       </c>
       <c r="D57" s="179" t="str">
-        <f>CONVENTIONS!$C$35 &amp;  " - " &amp; CONVENTIONS!AC5</f>
-        <v>Electricity - centralised</v>
+        <f>CONVENTIONS!$C$35 &amp;  " - " &amp; CONVENTIONS!AC7</f>
+        <v>Electricity - Centralised</v>
       </c>
       <c r="E57" s="174" t="s">
         <v>10</v>
@@ -24519,12 +24507,12 @@
         <v>23</v>
       </c>
       <c r="C58" s="179" t="str">
-        <f>CONVENTIONS!$B$35&amp;CONVENTIONS!AB6</f>
+        <f>CONVENTIONS!$B$35&amp;CONVENTIONS!AB8</f>
         <v>ELCD</v>
       </c>
       <c r="D58" s="179" t="str">
-        <f>CONVENTIONS!$C$35 &amp;  " - " &amp; CONVENTIONS!AC6</f>
-        <v>Electricity - decentralised</v>
+        <f>CONVENTIONS!$C$35 &amp;  " - " &amp; CONVENTIONS!AC8</f>
+        <v>Electricity - Distributed</v>
       </c>
       <c r="E58" s="174" t="s">
         <v>10</v>
@@ -24541,12 +24529,12 @@
         <v>23</v>
       </c>
       <c r="C59" s="179" t="str">
-        <f>CONVENTIONS!$P$5&amp;CONVENTIONS!$B$82&amp;CONVENTIONS!Y5&amp;CONVENTIONS!AB5</f>
-        <v>SUPH2GC</v>
+        <f>CONVENTIONS!$B$82</f>
+        <v>H2</v>
       </c>
       <c r="D59" s="179" t="str">
-        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z5 &amp; " - " &amp; CONVENTIONS!AC5&amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
-        <v>Hydrogen gaseous - centralised (SUP)</v>
+        <f>CONVENTIONS!$C$82</f>
+        <v>Hydrogen</v>
       </c>
       <c r="E59" s="174" t="s">
         <v>10</v>
@@ -24563,12 +24551,12 @@
         <v>23</v>
       </c>
       <c r="C60" s="179" t="str">
-        <f>CONVENTIONS!$P$5&amp;CONVENTIONS!$B$82&amp;CONVENTIONS!Y6&amp;CONVENTIONS!AB5</f>
-        <v>SUPH2LC</v>
+        <f>CONVENTIONS!$B$82&amp;CONVENTIONS!Y6</f>
+        <v>H2L</v>
       </c>
       <c r="D60" s="179" t="str">
-        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z6 &amp; " - " &amp; CONVENTIONS!AC5&amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
-        <v>Hydrogen liquid - centralised (SUP)</v>
+        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z6</f>
+        <v>Hydrogen liquid</v>
       </c>
       <c r="E60" s="174" t="s">
         <v>10</v>
@@ -24585,12 +24573,12 @@
         <v>23</v>
       </c>
       <c r="C61" s="179" t="str">
-        <f>CONVENTIONS!$P$5&amp;CONVENTIONS!$B$82&amp;CONVENTIONS!Y5&amp;CONVENTIONS!AB6</f>
-        <v>SUPH2GD</v>
+        <f>CONVENTIONS!$B$82&amp;CONVENTIONS!Y5&amp;CONVENTIONS!AB5</f>
+        <v>H2GH</v>
       </c>
       <c r="D61" s="179" t="str">
-        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z5 &amp; " - " &amp; CONVENTIONS!AC6 &amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
-        <v>Hydrogen gaseous - decentralised (SUP)</v>
+        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z5 &amp; " - " &amp; CONVENTIONS!AC5 &amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
+        <v>Hydrogen gaseous - High pressure (500 bar) (SUP)</v>
       </c>
       <c r="E61" s="174" t="s">
         <v>10</v>
@@ -24607,12 +24595,12 @@
         <v>23</v>
       </c>
       <c r="C62" s="179" t="str">
-        <f>CONVENTIONS!$P$5&amp;CONVENTIONS!$B$82&amp;CONVENTIONS!Y6&amp;CONVENTIONS!AB6</f>
-        <v>SUPH2LD</v>
+        <f>CONVENTIONS!$B$82&amp;CONVENTIONS!Y5&amp;CONVENTIONS!AB6</f>
+        <v>H2GM</v>
       </c>
       <c r="D62" s="179" t="str">
-        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z6 &amp; " - " &amp; CONVENTIONS!AC6 &amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
-        <v>Hydrogen liquid - decentralised (SUP)</v>
+        <f>CONVENTIONS!$C$82 &amp; " " &amp; CONVENTIONS!Z5 &amp; " - " &amp; CONVENTIONS!AC6 &amp; " (" &amp; CONVENTIONS!$P$5 &amp; ")"</f>
+        <v>Hydrogen gaseous - Medium pressure (100 bar) (SUP)</v>
       </c>
       <c r="E62" s="174" t="s">
         <v>10</v>
@@ -24847,27 +24835,27 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:T91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="58.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" customWidth="1"/>
+    <col min="8" max="8" width="30.3984375" customWidth="1"/>
+    <col min="9" max="9" width="25.3984375" customWidth="1"/>
+    <col min="10" max="10" width="17.3984375" customWidth="1"/>
+    <col min="14" max="14" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="26.25">
+    <row r="1" spans="2:10" ht="25.5">
       <c r="B1" s="175" t="s">
         <v>350</v>
       </c>
@@ -24893,12 +24881,12 @@
       <c r="I3" s="170"/>
       <c r="J3" s="170"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1">
+    <row r="4" spans="2:10" ht="14.65" thickBot="1">
       <c r="B4" s="166" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="166" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D4" s="166" t="s">
         <v>2</v>
@@ -24951,7 +24939,7 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="178" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C6" s="177"/>
       <c r="D6" s="177"/>
@@ -25369,7 +25357,7 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="177" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C22" s="177"/>
       <c r="D22" s="177"/>
@@ -25841,7 +25829,7 @@
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="177" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C40" s="177"/>
       <c r="D40" s="177"/>
@@ -27021,7 +27009,7 @@
         <v>10</v>
       </c>
       <c r="G83" s="186" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H83" s="167" t="s">
         <v>63</v>
@@ -27050,7 +27038,7 @@
         <v>10</v>
       </c>
       <c r="G84" s="186" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="H84" s="167" t="s">
         <v>63</v>
@@ -27253,278 +27241,278 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="11.5703125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="11.59765625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="23"/>
-    <col min="9" max="9" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="23" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="23"/>
-    <col min="13" max="13" width="11.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.1328125" style="23"/>
+    <col min="9" max="9" width="10.265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" style="23" customWidth="1"/>
+    <col min="12" max="12" width="9.1328125" style="23"/>
+    <col min="13" max="13" width="11.265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.73046875" style="23" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.85546875" style="23" customWidth="1"/>
-    <col min="18" max="262" width="9.140625" style="23"/>
-    <col min="263" max="263" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="266" max="518" width="9.140625" style="23"/>
-    <col min="519" max="519" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="521" max="521" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="522" max="774" width="9.140625" style="23"/>
-    <col min="775" max="775" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="777" max="777" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="778" max="1030" width="9.140625" style="23"/>
-    <col min="1031" max="1031" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="1033" max="1033" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1286" width="9.140625" style="23"/>
-    <col min="1287" max="1287" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="1289" max="1289" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="1290" max="1542" width="9.140625" style="23"/>
-    <col min="1543" max="1543" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="1545" max="1545" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="1546" max="1798" width="9.140625" style="23"/>
-    <col min="1799" max="1799" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="1801" max="1801" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="1802" max="2054" width="9.140625" style="23"/>
-    <col min="2055" max="2055" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2057" max="2057" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2058" max="2310" width="9.140625" style="23"/>
-    <col min="2311" max="2311" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2313" max="2313" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2314" max="2566" width="9.140625" style="23"/>
-    <col min="2567" max="2567" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2569" max="2569" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2570" max="2822" width="9.140625" style="23"/>
-    <col min="2823" max="2823" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="2825" max="2825" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2826" max="3078" width="9.140625" style="23"/>
-    <col min="3079" max="3079" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3081" max="3081" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3082" max="3334" width="9.140625" style="23"/>
-    <col min="3335" max="3335" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3337" max="3337" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3338" max="3590" width="9.140625" style="23"/>
-    <col min="3591" max="3591" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3593" max="3593" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3594" max="3846" width="9.140625" style="23"/>
-    <col min="3847" max="3847" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3849" max="3849" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3850" max="4102" width="9.140625" style="23"/>
-    <col min="4103" max="4103" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4105" max="4105" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4106" max="4358" width="9.140625" style="23"/>
-    <col min="4359" max="4359" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4361" max="4361" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4362" max="4614" width="9.140625" style="23"/>
-    <col min="4615" max="4615" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4617" max="4617" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4618" max="4870" width="9.140625" style="23"/>
-    <col min="4871" max="4871" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="4873" max="4873" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4874" max="5126" width="9.140625" style="23"/>
-    <col min="5127" max="5127" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5129" max="5129" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5382" width="9.140625" style="23"/>
-    <col min="5383" max="5383" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5385" max="5385" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5386" max="5638" width="9.140625" style="23"/>
-    <col min="5639" max="5639" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5641" max="5641" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5642" max="5894" width="9.140625" style="23"/>
-    <col min="5895" max="5895" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="5897" max="5897" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5898" max="6150" width="9.140625" style="23"/>
-    <col min="6151" max="6151" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6153" max="6153" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6154" max="6406" width="9.140625" style="23"/>
-    <col min="6407" max="6407" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6409" max="6409" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6410" max="6662" width="9.140625" style="23"/>
-    <col min="6663" max="6663" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6665" max="6665" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6666" max="6918" width="9.140625" style="23"/>
-    <col min="6919" max="6919" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6921" max="6921" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6922" max="7174" width="9.140625" style="23"/>
-    <col min="7175" max="7175" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7177" max="7177" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7178" max="7430" width="9.140625" style="23"/>
-    <col min="7431" max="7431" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7433" max="7433" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7434" max="7686" width="9.140625" style="23"/>
-    <col min="7687" max="7687" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7689" max="7689" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7690" max="7942" width="9.140625" style="23"/>
-    <col min="7943" max="7943" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7945" max="7945" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7946" max="8198" width="9.140625" style="23"/>
-    <col min="8199" max="8199" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="8201" max="8201" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8202" max="8454" width="9.140625" style="23"/>
-    <col min="8455" max="8455" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="8457" max="8457" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8458" max="8710" width="9.140625" style="23"/>
-    <col min="8711" max="8711" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="8713" max="8713" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8714" max="8966" width="9.140625" style="23"/>
-    <col min="8967" max="8967" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="8969" max="8969" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="8970" max="9222" width="9.140625" style="23"/>
-    <col min="9223" max="9223" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9225" max="9225" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9226" max="9478" width="9.140625" style="23"/>
-    <col min="9479" max="9479" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9481" max="9481" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9734" width="9.140625" style="23"/>
-    <col min="9735" max="9735" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9737" max="9737" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9738" max="9990" width="9.140625" style="23"/>
-    <col min="9991" max="9991" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9993" max="9993" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9994" max="10246" width="9.140625" style="23"/>
-    <col min="10247" max="10247" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10249" max="10249" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10250" max="10502" width="9.140625" style="23"/>
-    <col min="10503" max="10503" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10505" max="10505" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10506" max="10758" width="9.140625" style="23"/>
-    <col min="10759" max="10759" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="10761" max="10761" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10762" max="11014" width="9.140625" style="23"/>
-    <col min="11015" max="11015" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11017" max="11017" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11018" max="11270" width="9.140625" style="23"/>
-    <col min="11271" max="11271" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11273" max="11273" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11274" max="11526" width="9.140625" style="23"/>
-    <col min="11527" max="11527" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11529" max="11529" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11530" max="11782" width="9.140625" style="23"/>
-    <col min="11783" max="11783" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11785" max="11785" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11786" max="12038" width="9.140625" style="23"/>
-    <col min="12039" max="12039" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12041" max="12041" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12042" max="12294" width="9.140625" style="23"/>
-    <col min="12295" max="12295" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12297" max="12297" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12298" max="12550" width="9.140625" style="23"/>
-    <col min="12551" max="12551" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12553" max="12553" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12554" max="12806" width="9.140625" style="23"/>
-    <col min="12807" max="12807" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12809" max="12809" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12810" max="13062" width="9.140625" style="23"/>
-    <col min="13063" max="13063" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13065" max="13065" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13066" max="13318" width="9.140625" style="23"/>
-    <col min="13319" max="13319" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13321" max="13321" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13322" max="13574" width="9.140625" style="23"/>
-    <col min="13575" max="13575" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13577" max="13577" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13578" max="13830" width="9.140625" style="23"/>
-    <col min="13831" max="13831" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13833" max="13833" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13834" max="14086" width="9.140625" style="23"/>
-    <col min="14087" max="14087" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="14089" max="14089" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14090" max="14342" width="9.140625" style="23"/>
-    <col min="14343" max="14343" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="14345" max="14345" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14346" max="14598" width="9.140625" style="23"/>
-    <col min="14599" max="14599" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="14601" max="14601" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14602" max="14854" width="9.140625" style="23"/>
-    <col min="14855" max="14855" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="14857" max="14857" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14858" max="15110" width="9.140625" style="23"/>
-    <col min="15111" max="15111" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15113" max="15113" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="15114" max="15366" width="9.140625" style="23"/>
-    <col min="15367" max="15367" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15369" max="15369" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="15370" max="15622" width="9.140625" style="23"/>
-    <col min="15623" max="15623" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15625" max="15625" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="15626" max="15878" width="9.140625" style="23"/>
-    <col min="15879" max="15879" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="15881" max="15881" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="15882" max="16134" width="9.140625" style="23"/>
-    <col min="16135" max="16135" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="16137" max="16137" width="11.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="16138" max="16384" width="9.140625" style="23"/>
+    <col min="16" max="17" width="9.86328125" style="23" customWidth="1"/>
+    <col min="18" max="262" width="9.1328125" style="23"/>
+    <col min="263" max="263" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="266" max="518" width="9.1328125" style="23"/>
+    <col min="519" max="519" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="521" max="521" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="522" max="774" width="9.1328125" style="23"/>
+    <col min="775" max="775" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="777" max="777" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="778" max="1030" width="9.1328125" style="23"/>
+    <col min="1031" max="1031" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1033" max="1033" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1286" width="9.1328125" style="23"/>
+    <col min="1287" max="1287" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1289" max="1289" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1542" width="9.1328125" style="23"/>
+    <col min="1543" max="1543" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1545" max="1545" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1798" width="9.1328125" style="23"/>
+    <col min="1799" max="1799" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1801" max="1801" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1802" max="2054" width="9.1328125" style="23"/>
+    <col min="2055" max="2055" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2057" max="2057" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2310" width="9.1328125" style="23"/>
+    <col min="2311" max="2311" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2313" max="2313" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2566" width="9.1328125" style="23"/>
+    <col min="2567" max="2567" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2569" max="2569" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2822" width="9.1328125" style="23"/>
+    <col min="2823" max="2823" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2825" max="2825" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2826" max="3078" width="9.1328125" style="23"/>
+    <col min="3079" max="3079" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3081" max="3081" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3334" width="9.1328125" style="23"/>
+    <col min="3335" max="3335" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3337" max="3337" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3590" width="9.1328125" style="23"/>
+    <col min="3591" max="3591" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3593" max="3593" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3846" width="9.1328125" style="23"/>
+    <col min="3847" max="3847" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3849" max="3849" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3850" max="4102" width="9.1328125" style="23"/>
+    <col min="4103" max="4103" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4105" max="4105" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4358" width="9.1328125" style="23"/>
+    <col min="4359" max="4359" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4361" max="4361" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4614" width="9.1328125" style="23"/>
+    <col min="4615" max="4615" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4617" max="4617" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4870" width="9.1328125" style="23"/>
+    <col min="4871" max="4871" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4873" max="4873" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4874" max="5126" width="9.1328125" style="23"/>
+    <col min="5127" max="5127" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5129" max="5129" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5382" width="9.1328125" style="23"/>
+    <col min="5383" max="5383" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5385" max="5385" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5638" width="9.1328125" style="23"/>
+    <col min="5639" max="5639" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5641" max="5641" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5894" width="9.1328125" style="23"/>
+    <col min="5895" max="5895" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5897" max="5897" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5898" max="6150" width="9.1328125" style="23"/>
+    <col min="6151" max="6151" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6153" max="6153" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6406" width="9.1328125" style="23"/>
+    <col min="6407" max="6407" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6409" max="6409" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6662" width="9.1328125" style="23"/>
+    <col min="6663" max="6663" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6665" max="6665" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6918" width="9.1328125" style="23"/>
+    <col min="6919" max="6919" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6921" max="6921" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6922" max="7174" width="9.1328125" style="23"/>
+    <col min="7175" max="7175" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7177" max="7177" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7430" width="9.1328125" style="23"/>
+    <col min="7431" max="7431" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7433" max="7433" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7686" width="9.1328125" style="23"/>
+    <col min="7687" max="7687" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7689" max="7689" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7942" width="9.1328125" style="23"/>
+    <col min="7943" max="7943" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7945" max="7945" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7946" max="8198" width="9.1328125" style="23"/>
+    <col min="8199" max="8199" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8201" max="8201" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8454" width="9.1328125" style="23"/>
+    <col min="8455" max="8455" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8457" max="8457" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8710" width="9.1328125" style="23"/>
+    <col min="8711" max="8711" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8713" max="8713" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8966" width="9.1328125" style="23"/>
+    <col min="8967" max="8967" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8969" max="8969" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8970" max="9222" width="9.1328125" style="23"/>
+    <col min="9223" max="9223" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9225" max="9225" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9478" width="9.1328125" style="23"/>
+    <col min="9479" max="9479" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9481" max="9481" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9734" width="9.1328125" style="23"/>
+    <col min="9735" max="9735" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9737" max="9737" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9990" width="9.1328125" style="23"/>
+    <col min="9991" max="9991" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9993" max="9993" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9994" max="10246" width="9.1328125" style="23"/>
+    <col min="10247" max="10247" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10249" max="10249" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10502" width="9.1328125" style="23"/>
+    <col min="10503" max="10503" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10505" max="10505" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10758" width="9.1328125" style="23"/>
+    <col min="10759" max="10759" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10761" max="10761" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10762" max="11014" width="9.1328125" style="23"/>
+    <col min="11015" max="11015" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11017" max="11017" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11270" width="9.1328125" style="23"/>
+    <col min="11271" max="11271" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11273" max="11273" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11526" width="9.1328125" style="23"/>
+    <col min="11527" max="11527" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11529" max="11529" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11782" width="9.1328125" style="23"/>
+    <col min="11783" max="11783" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11785" max="11785" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="11786" max="12038" width="9.1328125" style="23"/>
+    <col min="12039" max="12039" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12041" max="12041" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12294" width="9.1328125" style="23"/>
+    <col min="12295" max="12295" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12297" max="12297" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12550" width="9.1328125" style="23"/>
+    <col min="12551" max="12551" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12553" max="12553" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12806" width="9.1328125" style="23"/>
+    <col min="12807" max="12807" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12809" max="12809" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12810" max="13062" width="9.1328125" style="23"/>
+    <col min="13063" max="13063" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13065" max="13065" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13318" width="9.1328125" style="23"/>
+    <col min="13319" max="13319" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13321" max="13321" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13574" width="9.1328125" style="23"/>
+    <col min="13575" max="13575" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13577" max="13577" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13830" width="9.1328125" style="23"/>
+    <col min="13831" max="13831" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13833" max="13833" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13834" max="14086" width="9.1328125" style="23"/>
+    <col min="14087" max="14087" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14089" max="14089" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14342" width="9.1328125" style="23"/>
+    <col min="14343" max="14343" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14345" max="14345" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14598" width="9.1328125" style="23"/>
+    <col min="14599" max="14599" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14601" max="14601" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14854" width="9.1328125" style="23"/>
+    <col min="14855" max="14855" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14857" max="14857" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="14858" max="15110" width="9.1328125" style="23"/>
+    <col min="15111" max="15111" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15113" max="15113" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15366" width="9.1328125" style="23"/>
+    <col min="15367" max="15367" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15369" max="15369" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15622" width="9.1328125" style="23"/>
+    <col min="15623" max="15623" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15625" max="15625" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15878" width="9.1328125" style="23"/>
+    <col min="15879" max="15879" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15881" max="15881" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="15882" max="16134" width="9.1328125" style="23"/>
+    <col min="16135" max="16135" width="10.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="14.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="16137" max="16137" width="11.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="18.75">
+    <row r="1" spans="2:19" ht="18">
       <c r="B1" s="154" t="s">
         <v>224</v>
       </c>
@@ -27541,7 +27529,7 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="157" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C4" s="157" t="s">
         <v>2</v>
@@ -27562,7 +27550,7 @@
         <v>225</v>
       </c>
       <c r="I4" s="158" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J4" s="158" t="s">
         <v>226</v>
@@ -27571,7 +27559,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="15.75" thickBot="1">
+    <row r="5" spans="2:19" ht="14.65" thickBot="1">
       <c r="B5" s="159" t="s">
         <v>211</v>
       </c>
@@ -27785,39 +27773,39 @@
       <selection activeCell="K42" sqref="K42:L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="12.5703125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="23" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="23" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="23" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="23" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="23" customWidth="1"/>
-    <col min="16" max="22" width="9.140625" style="23"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="12.59765625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="23.265625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.86328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1328125" style="23" customWidth="1"/>
+    <col min="12" max="12" width="12.73046875" style="23" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" style="23" customWidth="1"/>
+    <col min="14" max="14" width="15.1328125" style="23" customWidth="1"/>
+    <col min="15" max="15" width="10.59765625" style="23" customWidth="1"/>
+    <col min="16" max="22" width="9.1328125" style="23"/>
     <col min="23" max="23" width="16" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" style="23" customWidth="1"/>
-    <col min="25" max="25" width="38.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="23"/>
+    <col min="24" max="24" width="19.3984375" style="23" customWidth="1"/>
+    <col min="25" max="25" width="38.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="18.75">
+    <row r="1" spans="2:20" ht="18">
       <c r="B1" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="3" spans="2:20" ht="18.75">
+    <row r="3" spans="2:20" ht="18">
       <c r="G3" s="257" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="5"/>
@@ -27833,45 +27821,45 @@
     </row>
     <row r="4" spans="2:20">
       <c r="C4" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>603</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>604</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>605</v>
       </c>
       <c r="N4" s="38" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="26.25" thickBot="1">
+    <row r="5" spans="2:20" ht="26.65" thickBot="1">
       <c r="C5" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>46</v>
@@ -27880,7 +27868,7 @@
         <v>47</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>48</v>
@@ -27948,7 +27936,7 @@
         <v>13.293106237838872</v>
       </c>
       <c r="N6" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="2:20">
@@ -27996,13 +27984,13 @@
         <v>12.890088334941915</v>
       </c>
       <c r="N7" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="T7" s="23" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="2:20">
@@ -28050,7 +28038,7 @@
         <v>2.065279967615445</v>
       </c>
       <c r="N8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="9" spans="2:20">
@@ -28101,10 +28089,10 @@
         <v>0.95000000000000495</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="S9" s="23" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -28155,7 +28143,7 @@
         <v>1.2700000000000062</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="S10" s="23">
         <v>58.93</v>
@@ -28209,7 +28197,7 @@
         <v>0.87557603686636576</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="S11" s="23">
         <v>19.86</v>
@@ -28263,7 +28251,7 @@
         <v>1.0669585115925122</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="S12" s="23">
         <v>102.22</v>
@@ -28692,30 +28680,30 @@
     </row>
     <row r="24" spans="3:21">
       <c r="C24" s="245" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D24" s="246"/>
       <c r="E24" s="246"/>
       <c r="F24" s="247"/>
       <c r="G24" s="442" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H24" s="442"/>
       <c r="I24" s="442"/>
       <c r="J24" s="443"/>
       <c r="K24" s="444" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L24" s="445"/>
       <c r="M24" s="446" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N24" s="445"/>
       <c r="S24"/>
     </row>
     <row r="25" spans="3:21">
       <c r="C25" s="241" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D25" s="241" t="s">
         <v>76</v>
@@ -28754,10 +28742,10 @@
     </row>
     <row r="26" spans="3:21">
       <c r="C26" s="233" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D26" s="233" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E26" s="235">
         <v>91</v>
@@ -28793,10 +28781,10 @@
     </row>
     <row r="27" spans="3:21">
       <c r="C27" s="233" t="s">
+        <v>517</v>
+      </c>
+      <c r="D27" s="233" t="s">
         <v>519</v>
-      </c>
-      <c r="D27" s="233" t="s">
-        <v>521</v>
       </c>
       <c r="E27" s="235">
         <v>8.6999999999999993</v>
@@ -28833,10 +28821,10 @@
     </row>
     <row r="28" spans="3:21">
       <c r="C28" s="237" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D28" s="237" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E28" s="239">
         <v>108</v>
@@ -28873,7 +28861,7 @@
     </row>
     <row r="29" spans="3:21">
       <c r="C29" s="30" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29"/>
@@ -28905,7 +28893,7 @@
     </row>
     <row r="31" spans="3:21">
       <c r="C31" s="254" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D31" s="254"/>
       <c r="E31" s="258">
@@ -28956,7 +28944,7 @@
         <v xml:space="preserve">IEA crude oil </v>
       </c>
       <c r="D32" s="256" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E32" s="251">
         <f>E26/Conversions!$C$10</f>
@@ -29006,7 +28994,7 @@
         <v>Natural Gas - EU</v>
       </c>
       <c r="D33" s="234" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E33" s="248">
         <f>E27/Conversions!$C$10</f>
@@ -29056,7 +29044,7 @@
         <v>Steam coal - EU</v>
       </c>
       <c r="D34" s="238" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E34" s="253">
         <f>E28/Conversions!$C$10</f>
@@ -29117,7 +29105,7 @@
     </row>
     <row r="36" spans="3:20">
       <c r="C36" s="254" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D36" s="254"/>
       <c r="E36" s="258">
@@ -29168,7 +29156,7 @@
         <v xml:space="preserve">IEA crude oil </v>
       </c>
       <c r="D37" s="256" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E37" s="251">
         <f>E32/Conversions!$C$5</f>
@@ -29218,7 +29206,7 @@
         <v>Natural Gas - EU</v>
       </c>
       <c r="D38" s="234" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E38" s="248">
         <f>E33/Conversions!$C$3</f>
@@ -29268,7 +29256,7 @@
         <v>Steam coal - EU</v>
       </c>
       <c r="D39" s="238" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E39" s="253">
         <f>E34/(Conversions!$C$2*1000)</f>
@@ -29348,30 +29336,30 @@
     </row>
     <row r="42" spans="3:20">
       <c r="C42" s="245" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D42" s="246"/>
       <c r="E42" s="246"/>
       <c r="F42" s="247"/>
       <c r="G42" s="442" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H42" s="442"/>
       <c r="I42" s="442"/>
       <c r="J42" s="443"/>
       <c r="K42" s="444" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="L42" s="445"/>
       <c r="M42" s="446" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="N42" s="445"/>
       <c r="O42"/>
     </row>
     <row r="43" spans="3:20">
       <c r="C43" s="241" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D43" s="241" t="s">
         <v>76</v>
@@ -29410,10 +29398,10 @@
     </row>
     <row r="44" spans="3:20">
       <c r="C44" s="233" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D44" s="233" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E44" s="235">
         <v>90</v>
@@ -29451,10 +29439,10 @@
     </row>
     <row r="45" spans="3:20">
       <c r="C45" s="233" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D45" s="233" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E45" s="235">
         <v>8.6</v>
@@ -29492,10 +29480,10 @@
     </row>
     <row r="46" spans="3:20">
       <c r="C46" s="237" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D46" s="237" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E46" s="239">
         <v>106</v>
@@ -29533,7 +29521,7 @@
     </row>
     <row r="47" spans="3:20">
       <c r="C47" s="30" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D47" s="34"/>
       <c r="E47"/>
@@ -29569,7 +29557,7 @@
     </row>
     <row r="49" spans="3:20">
       <c r="C49" s="254" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D49" s="254"/>
       <c r="E49" s="258">
@@ -29622,7 +29610,7 @@
         <v xml:space="preserve">IEA crude oil </v>
       </c>
       <c r="D50" s="256" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E50" s="251">
         <f>E44/Conversions!$C$11</f>
@@ -29674,7 +29662,7 @@
         <v>Natural Gas - EU</v>
       </c>
       <c r="D51" s="234" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E51" s="248">
         <f>E45/Conversions!$C$11</f>
@@ -29726,7 +29714,7 @@
         <v>Steam coal - EU</v>
       </c>
       <c r="D52" s="238" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E52" s="253">
         <f>E46/Conversions!$C$11</f>
@@ -29791,7 +29779,7 @@
     </row>
     <row r="54" spans="3:20">
       <c r="C54" s="254" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D54" s="254"/>
       <c r="E54" s="258">
@@ -29843,7 +29831,7 @@
         <v xml:space="preserve">IEA crude oil </v>
       </c>
       <c r="D55" s="256" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E55" s="251">
         <f>E50/Conversions!$C$5</f>
@@ -29894,7 +29882,7 @@
         <v>Natural Gas - EU</v>
       </c>
       <c r="D56" s="234" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E56" s="248">
         <f>E51/Conversions!$C$3</f>
@@ -29945,7 +29933,7 @@
         <v>Steam coal - EU</v>
       </c>
       <c r="D57" s="238" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E57" s="253">
         <f>E52/(Conversions!$C$2*1000)</f>
@@ -30188,31 +30176,31 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="23"/>
-    <col min="2" max="2" width="14.28515625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="12.85546875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="23"/>
+    <col min="2" max="2" width="14.265625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.73046875" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="12.86328125" style="23" customWidth="1"/>
     <col min="15" max="16" width="13" style="23" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" style="23" customWidth="1"/>
-    <col min="18" max="18" width="29.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="9.140625" style="23"/>
-    <col min="23" max="23" width="14.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="23"/>
+    <col min="17" max="17" width="21.86328125" style="23" customWidth="1"/>
+    <col min="18" max="18" width="29.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="9.1328125" style="23"/>
+    <col min="23" max="23" width="14.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.59765625" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.1328125" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="18.75">
+    <row r="2" spans="2:12" ht="18">
       <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F2" s="92"/>
       <c r="G2" s="92"/>
@@ -30224,13 +30212,13 @@
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>38</v>
@@ -30259,7 +30247,7 @@
     </row>
     <row r="4" spans="2:12" ht="32.450000000000003" customHeight="1" thickBot="1">
       <c r="B4" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>59</v>
@@ -30931,7 +30919,7 @@
       <c r="K21" s="50"/>
       <c r="L21" s="22"/>
     </row>
-    <row r="22" spans="2:18" ht="18.75">
+    <row r="22" spans="2:18" ht="18">
       <c r="B22" s="3" t="s">
         <v>81</v>
       </c>
@@ -30951,16 +30939,16 @@
     </row>
     <row r="23" spans="2:18" ht="30.75" customHeight="1">
       <c r="B23" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>38</v>
@@ -30993,9 +30981,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="26.25" thickBot="1">
+    <row r="24" spans="2:18" ht="26.65" thickBot="1">
       <c r="B24" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>59</v>
@@ -31004,7 +30992,7 @@
         <v>47</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>48</v>
@@ -31074,7 +31062,7 @@
         <v>35.031244673834173</v>
       </c>
       <c r="M25" s="270" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -31091,14 +31079,14 @@
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
     </row>
-    <row r="27" spans="2:18" ht="26.25">
+    <row r="27" spans="2:18" ht="25.5">
       <c r="B27" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="22"/>
@@ -31117,13 +31105,13 @@
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>38</v>
@@ -31150,9 +31138,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="2:18" ht="15.75" thickBot="1">
+    <row r="29" spans="2:18" ht="14.65" thickBot="1">
       <c r="B29" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>59</v>
@@ -31189,7 +31177,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="15.75" thickBot="1">
+    <row r="30" spans="2:18" ht="14.65" thickBot="1">
       <c r="B30" s="43" t="str">
         <f t="shared" ref="B30" si="0">B13</f>
         <v>IE,National</v>
@@ -31548,7 +31536,7 @@
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
     </row>
-    <row r="40" spans="2:23" ht="18.75">
+    <row r="40" spans="2:23" ht="18">
       <c r="B40" s="3" t="s">
         <v>82</v>
       </c>
@@ -31570,13 +31558,13 @@
     </row>
     <row r="41" spans="2:23">
       <c r="B41" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>38</v>
@@ -31619,9 +31607,9 @@
       <c r="V41"/>
       <c r="W41"/>
     </row>
-    <row r="42" spans="2:23" ht="15.75" thickBot="1">
+    <row r="42" spans="2:23" ht="14.65" thickBot="1">
       <c r="B42" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>59</v>
@@ -31657,7 +31645,7 @@
         <v>10</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
@@ -31721,7 +31709,7 @@
         <v>5</v>
       </c>
       <c r="O43" s="61" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="P43" s="52"/>
       <c r="R43"/>
@@ -31910,7 +31898,7 @@
       <c r="V46"/>
       <c r="W46"/>
     </row>
-    <row r="47" spans="2:23" ht="15.75" thickBot="1">
+    <row r="47" spans="2:23" ht="14.65" thickBot="1">
       <c r="B47" s="46" t="s">
         <v>79</v>
       </c>
@@ -32011,7 +31999,7 @@
         <v>5</v>
       </c>
       <c r="O48" s="61" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="P48" s="52"/>
       <c r="R48"/>
@@ -32192,7 +32180,7 @@
       <c r="P51" s="51"/>
       <c r="R51" s="25"/>
     </row>
-    <row r="52" spans="2:18" ht="15.75" thickBot="1">
+    <row r="52" spans="2:18" ht="14.65" thickBot="1">
       <c r="B52" s="46" t="s">
         <v>79</v>
       </c>
@@ -32466,7 +32454,7 @@
       <c r="P56" s="51"/>
       <c r="R56" s="25"/>
     </row>
-    <row r="57" spans="2:18" ht="15.75" thickBot="1">
+    <row r="57" spans="2:18" ht="14.65" thickBot="1">
       <c r="B57" s="46" t="s">
         <v>79</v>
       </c>
@@ -32741,7 +32729,7 @@
       <c r="P61" s="51"/>
       <c r="R61" s="25"/>
     </row>
-    <row r="62" spans="2:18" ht="15.75" thickBot="1">
+    <row r="62" spans="2:18" ht="14.65" thickBot="1">
       <c r="B62" s="48" t="s">
         <v>79</v>
       </c>
@@ -32793,21 +32781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -32953,31 +32926,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F399E6-2CA4-4BC3-AE7C-3570BA9F00A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F32A5943-069C-47E6-B7B1-1C4E8CC11B6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32993,4 +32957,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F399E6-2CA4-4BC3-AE7C-3570BA9F00A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1EBC224-6025-40B6-954C-A60FF473B45B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>